<commit_message>
feat: integrate sunset calculations and update weather icon logic based on sunrise/sunset times
</commit_message>
<xml_diff>
--- a/docs/cwa_weather_code_to_mdi_icon_mapping_table.xlsx
+++ b/docs/cwa_weather_code_to_mdi_icon_mapping_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\github\esphome-cwa-town-forecast\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30C2FAF-D4BC-4008-B42A-E2FFC28BEB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC00B55-D751-4DA5-A274-89958ED9AC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E8F7E36D-7476-4FAD-A608-6F16C0C39392}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="125">
   <si>
     <t>圖示名稱</t>
   </si>
@@ -428,6 +428,10 @@
   </si>
   <si>
     <t>F0594</t>
+  </si>
+  <si>
+    <t>MDI Icon Name(Sunset - Sunrise)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -827,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FEDE8E-0F93-493C-AF41-1E26857B4B38}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -841,9 +845,12 @@
     <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="60" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="63.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -862,8 +869,17 @@
       <c r="F1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -884,8 +900,19 @@
         <f>VLOOKUP(D2,工作表1!$A$1:$C$12, 3, 0)</f>
         <v>https://pictogrammers.com/library/mdi/icon/weather-sunny/</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" t="str">
+        <f>VLOOKUP(G2,工作表1!$A$2:$C$14,2,0)</f>
+        <v>F0594</v>
+      </c>
+      <c r="I2" t="str">
+        <f>VLOOKUP(G2,工作表1!$A$2:$C$14,3,0)</f>
+        <v>https://pictogrammers.com/library/mdi/icon/weather-night/</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -906,8 +933,19 @@
         <f>VLOOKUP(D3,工作表1!$A$1:$C$12, 3, 0)</f>
         <v>https://pictogrammers.com/library/mdi/icon/weather-partly-cloudy/</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" t="str">
+        <f>VLOOKUP(G3,工作表1!$A$2:$C$14,2,0)</f>
+        <v>F0F31</v>
+      </c>
+      <c r="I3" t="str">
+        <f>VLOOKUP(G3,工作表1!$A$2:$C$14,3,0)</f>
+        <v>https://pictogrammers.com/library/mdi/icon/weather-night-partly-cloudy/</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -928,8 +966,19 @@
         <f>VLOOKUP(D4,工作表1!$A$1:$C$12, 3, 0)</f>
         <v>https://pictogrammers.com/library/mdi/icon/weather-partly-cloudy/</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" t="str">
+        <f>VLOOKUP(G4,工作表1!$A$2:$C$14,2,0)</f>
+        <v>F0F31</v>
+      </c>
+      <c r="I4" t="str">
+        <f>VLOOKUP(G4,工作表1!$A$2:$C$14,3,0)</f>
+        <v>https://pictogrammers.com/library/mdi/icon/weather-night-partly-cloudy/</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -950,8 +999,19 @@
         <f>VLOOKUP(D5,工作表1!$A$1:$C$12, 3, 0)</f>
         <v>https://pictogrammers.com/library/mdi/icon/weather-partly-cloudy/</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" t="str">
+        <f>VLOOKUP(G5,工作表1!$A$2:$C$14,2,0)</f>
+        <v>F0F31</v>
+      </c>
+      <c r="I5" t="str">
+        <f>VLOOKUP(G5,工作表1!$A$2:$C$14,3,0)</f>
+        <v>https://pictogrammers.com/library/mdi/icon/weather-night-partly-cloudy/</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -972,8 +1032,19 @@
         <f>VLOOKUP(D6,工作表1!$A$1:$C$12, 3, 0)</f>
         <v>https://pictogrammers.com/library/mdi/icon/weather-cloudy/</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" t="str">
+        <f>VLOOKUP(G6,工作表1!$A$2:$C$14,2,0)</f>
+        <v>F0F31</v>
+      </c>
+      <c r="I6" t="str">
+        <f>VLOOKUP(G6,工作表1!$A$2:$C$14,3,0)</f>
+        <v>https://pictogrammers.com/library/mdi/icon/weather-night-partly-cloudy/</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -994,8 +1065,19 @@
         <f>VLOOKUP(D7,工作表1!$A$1:$C$12, 3, 0)</f>
         <v>https://pictogrammers.com/library/mdi/icon/weather-cloudy/</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" t="str">
+        <f>VLOOKUP(G7,工作表1!$A$2:$C$14,2,0)</f>
+        <v>F0F31</v>
+      </c>
+      <c r="I7" t="str">
+        <f>VLOOKUP(G7,工作表1!$A$2:$C$14,3,0)</f>
+        <v>https://pictogrammers.com/library/mdi/icon/weather-night-partly-cloudy/</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1016,8 +1098,19 @@
         <f>VLOOKUP(D8,工作表1!$A$1:$C$12, 3, 0)</f>
         <v>https://pictogrammers.com/library/mdi/icon/weather-cloudy/</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" t="str">
+        <f>VLOOKUP(G8,工作表1!$A$2:$C$14,2,0)</f>
+        <v>F0F31</v>
+      </c>
+      <c r="I8" t="str">
+        <f>VLOOKUP(G8,工作表1!$A$2:$C$14,3,0)</f>
+        <v>https://pictogrammers.com/library/mdi/icon/weather-night-partly-cloudy/</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1039,7 +1132,7 @@
         <v>https://pictogrammers.com/library/mdi/icon/weather-pouring/</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1061,7 +1154,7 @@
         <v>https://pictogrammers.com/library/mdi/icon/weather-partly-rainy/</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1083,7 +1176,7 @@
         <v>https://pictogrammers.com/library/mdi/icon/weather-partly-rainy/</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1105,7 +1198,7 @@
         <v>https://pictogrammers.com/library/mdi/icon/weather-rainy/</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1127,7 +1220,7 @@
         <v>https://pictogrammers.com/library/mdi/icon/weather-rainy/</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1149,7 +1242,7 @@
         <v>https://pictogrammers.com/library/mdi/icon/weather-rainy/</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1171,7 +1264,7 @@
         <v>https://pictogrammers.com/library/mdi/icon/weather-rainy/</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1777,7 +1870,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>

</xml_diff>